<commit_message>
Auto-committed on 2022/02/18 週五
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/L4-批次作業/AchAuthLog.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/L4-批次作業/AchAuthLog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\SKL\DB\GenTables\L4-批次作業\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\SKL\DB\GenTables\L4-批次作業\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C9E0AD6-3712-459C-8EE8-9A2A4F39DC04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{027263A6-421E-4418-9942-292E5A72ABD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DBD" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="219">
   <si>
     <t>SEQ</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -703,10 +703,6 @@
   <si>
     <t>A：新增(人工紙本)
 O：舊檔轉換用</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <t>OccAuthCreateDate</t>
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
@@ -924,6 +920,25 @@
 1:需審查/確認
 2:為凍結名單/未確定名單</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>資料製作日期</t>
+  </si>
+  <si>
+    <t>OccPropDate</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>提出日期(西元)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CustNo = ,AND FacmNo = ,AND RepayBank = ,AND RepayAcct = ,AND PropDate = </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>facmNoPropDateFirst</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1607,7 +1622,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
@@ -1841,7 +1856,7 @@
         <v>1</v>
       </c>
       <c r="G14" s="21" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1921,7 +1936,7 @@
         <v>1</v>
       </c>
       <c r="G18" s="21" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="48.6">
@@ -1941,7 +1956,7 @@
         <v>1</v>
       </c>
       <c r="G19" s="21" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1984,7 +1999,7 @@
         <v>1</v>
       </c>
       <c r="G21" s="21" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -2046,10 +2061,10 @@
         <v>16</v>
       </c>
       <c r="B25" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="C25" s="24" t="s">
         <v>197</v>
-      </c>
-      <c r="C25" s="24" t="s">
-        <v>198</v>
       </c>
       <c r="D25" s="25" t="s">
         <v>74</v>
@@ -2058,7 +2073,7 @@
         <v>8</v>
       </c>
       <c r="G25" s="20" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="226.8">
@@ -2078,7 +2093,7 @@
         <v>2</v>
       </c>
       <c r="G26" s="21" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -2152,7 +2167,7 @@
         <v>1</v>
       </c>
       <c r="G30" s="20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="64.8">
@@ -2172,7 +2187,7 @@
         <v>1</v>
       </c>
       <c r="G31" s="27" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -2180,10 +2195,10 @@
         <v>23</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C32" s="24" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D32" s="22" t="s">
         <v>32</v>
@@ -2280,11 +2295,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2"/>
@@ -2445,7 +2460,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>118</v>
@@ -2467,21 +2482,29 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>208</v>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -2495,8 +2518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2"/>
@@ -2864,10 +2887,10 @@
         <v>9</v>
       </c>
       <c r="B16" s="34" t="s">
+        <v>215</v>
+      </c>
+      <c r="C16" s="34" t="s">
         <v>171</v>
-      </c>
-      <c r="C16" s="34" t="s">
-        <v>172</v>
       </c>
       <c r="D16" s="34">
         <v>9</v>
@@ -2878,7 +2901,9 @@
       <c r="F16" s="34">
         <v>79</v>
       </c>
-      <c r="G16" s="35"/>
+      <c r="G16" s="35" t="s">
+        <v>216</v>
+      </c>
       <c r="H16" s="33"/>
     </row>
     <row r="17" spans="1:8">
@@ -2886,10 +2911,10 @@
         <v>10</v>
       </c>
       <c r="B17" s="34" t="s">
+        <v>172</v>
+      </c>
+      <c r="C17" s="34" t="s">
         <v>173</v>
-      </c>
-      <c r="C17" s="34" t="s">
-        <v>174</v>
       </c>
       <c r="D17" s="34">
         <v>9</v>
@@ -2901,7 +2926,7 @@
         <v>86</v>
       </c>
       <c r="G17" s="35" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H17" s="33"/>
     </row>
@@ -2910,10 +2935,10 @@
         <v>11</v>
       </c>
       <c r="B18" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C18" s="34" t="s">
         <v>176</v>
-      </c>
-      <c r="C18" s="34" t="s">
-        <v>177</v>
       </c>
       <c r="D18" s="34" t="s">
         <v>134</v>
@@ -2925,7 +2950,7 @@
         <v>106</v>
       </c>
       <c r="G18" s="35" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H18" s="33"/>
     </row>
@@ -2934,10 +2959,10 @@
         <v>12</v>
       </c>
       <c r="B19" s="34" t="s">
+        <v>178</v>
+      </c>
+      <c r="C19" s="34" t="s">
         <v>179</v>
-      </c>
-      <c r="C19" s="34" t="s">
-        <v>180</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>134</v>
@@ -2949,7 +2974,7 @@
         <v>107</v>
       </c>
       <c r="G19" s="35" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H19" s="33"/>
     </row>
@@ -2958,10 +2983,10 @@
         <v>13</v>
       </c>
       <c r="B20" s="34" t="s">
+        <v>181</v>
+      </c>
+      <c r="C20" s="34" t="s">
         <v>182</v>
-      </c>
-      <c r="C20" s="34" t="s">
-        <v>183</v>
       </c>
       <c r="D20" s="34" t="s">
         <v>134</v>
@@ -2973,7 +2998,7 @@
         <v>108</v>
       </c>
       <c r="G20" s="35" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H20" s="33"/>
     </row>
@@ -2982,10 +3007,10 @@
         <v>14</v>
       </c>
       <c r="B21" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="C21" s="34" t="s">
         <v>185</v>
-      </c>
-      <c r="C21" s="34" t="s">
-        <v>186</v>
       </c>
       <c r="D21" s="34" t="s">
         <v>134</v>
@@ -3004,7 +3029,7 @@
         <v>15</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C22" s="34" t="s">
         <v>147</v>
@@ -3036,10 +3061,10 @@
         <v>1</v>
       </c>
       <c r="B24" s="34" t="s">
+        <v>187</v>
+      </c>
+      <c r="C24" s="34" t="s">
         <v>188</v>
-      </c>
-      <c r="C24" s="34" t="s">
-        <v>189</v>
       </c>
       <c r="D24" s="34" t="s">
         <v>134</v>
@@ -3051,7 +3076,7 @@
         <v>3</v>
       </c>
       <c r="G24" s="35" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H24" s="33"/>
     </row>
@@ -3060,10 +3085,10 @@
         <v>2</v>
       </c>
       <c r="B25" s="34" t="s">
+        <v>190</v>
+      </c>
+      <c r="C25" s="34" t="s">
         <v>191</v>
-      </c>
-      <c r="C25" s="34" t="s">
-        <v>192</v>
       </c>
       <c r="D25" s="34">
         <v>9</v>
@@ -3082,7 +3107,7 @@
         <v>3</v>
       </c>
       <c r="B26" s="34" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C26" s="34" t="s">
         <v>147</v>
@@ -3109,8 +3134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2"/>
@@ -3143,7 +3168,7 @@
         <v>128</v>
       </c>
       <c r="F1" s="28" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G1" s="28" t="s">
         <v>129</v>
@@ -3152,7 +3177,7 @@
         <v>130</v>
       </c>
       <c r="I1" s="30" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -3533,10 +3558,10 @@
         <v>9</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>171</v>
+        <v>215</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>172</v>
+        <v>214</v>
       </c>
       <c r="D16" s="34">
         <v>9</v>
@@ -3551,7 +3576,9 @@
       <c r="G16" s="34">
         <v>79</v>
       </c>
-      <c r="H16" s="35"/>
+      <c r="H16" s="35" t="s">
+        <v>216</v>
+      </c>
       <c r="I16" s="33"/>
     </row>
     <row r="17" spans="1:9">
@@ -3559,10 +3586,10 @@
         <v>10</v>
       </c>
       <c r="B17" s="34" t="s">
+        <v>172</v>
+      </c>
+      <c r="C17" s="34" t="s">
         <v>173</v>
-      </c>
-      <c r="C17" s="34" t="s">
-        <v>174</v>
       </c>
       <c r="D17" s="34">
         <v>9</v>
@@ -3578,7 +3605,7 @@
         <v>86</v>
       </c>
       <c r="H17" s="35" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I17" s="33"/>
     </row>
@@ -3587,10 +3614,10 @@
         <v>11</v>
       </c>
       <c r="B18" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C18" s="34" t="s">
         <v>176</v>
-      </c>
-      <c r="C18" s="34" t="s">
-        <v>177</v>
       </c>
       <c r="D18" s="34" t="s">
         <v>134</v>
@@ -3606,7 +3633,7 @@
         <v>106</v>
       </c>
       <c r="H18" s="35" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I18" s="33"/>
     </row>
@@ -3615,10 +3642,10 @@
         <v>12</v>
       </c>
       <c r="B19" s="34" t="s">
+        <v>178</v>
+      </c>
+      <c r="C19" s="34" t="s">
         <v>179</v>
-      </c>
-      <c r="C19" s="34" t="s">
-        <v>180</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>134</v>
@@ -3634,10 +3661,10 @@
         <v>107</v>
       </c>
       <c r="H19" s="38" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I19" s="38" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -3645,10 +3672,10 @@
         <v>13</v>
       </c>
       <c r="B20" s="34" t="s">
+        <v>181</v>
+      </c>
+      <c r="C20" s="34" t="s">
         <v>182</v>
-      </c>
-      <c r="C20" s="34" t="s">
-        <v>183</v>
       </c>
       <c r="D20" s="34" t="s">
         <v>134</v>
@@ -3664,7 +3691,7 @@
         <v>108</v>
       </c>
       <c r="H20" s="35" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I20" s="33"/>
     </row>
@@ -3673,10 +3700,10 @@
         <v>14</v>
       </c>
       <c r="B21" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="C21" s="34" t="s">
         <v>185</v>
-      </c>
-      <c r="C21" s="34" t="s">
-        <v>186</v>
       </c>
       <c r="D21" s="34" t="s">
         <v>134</v>
@@ -3699,7 +3726,7 @@
         <v>15</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C22" s="34" t="s">
         <v>147</v>
@@ -3736,10 +3763,10 @@
         <v>1</v>
       </c>
       <c r="B24" s="34" t="s">
+        <v>187</v>
+      </c>
+      <c r="C24" s="34" t="s">
         <v>188</v>
-      </c>
-      <c r="C24" s="34" t="s">
-        <v>189</v>
       </c>
       <c r="D24" s="34" t="s">
         <v>134</v>
@@ -3754,7 +3781,7 @@
         <v>3</v>
       </c>
       <c r="H24" s="35" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I24" s="33"/>
     </row>
@@ -3763,10 +3790,10 @@
         <v>2</v>
       </c>
       <c r="B25" s="34" t="s">
+        <v>190</v>
+      </c>
+      <c r="C25" s="34" t="s">
         <v>191</v>
-      </c>
-      <c r="C25" s="34" t="s">
-        <v>192</v>
       </c>
       <c r="D25" s="34">
         <v>9</v>
@@ -3789,7 +3816,7 @@
         <v>3</v>
       </c>
       <c r="B26" s="34" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C26" s="34" t="s">
         <v>147</v>

</xml_diff>